<commit_message>
update readme and results
</commit_message>
<xml_diff>
--- a/androidworld_eval_result/androidworld_result.xlsx
+++ b/androidworld_eval_result/androidworld_result.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20417"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspace\ui_tars\android_world\androidworld_eval_result\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspace\LX-GUIAgent\0.79\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2FFD4E8-39C5-4EAC-9D58-93B397C5B8EB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{05BF3FED-9C42-4A09-84AC-4CF6F4958B50}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15105" windowHeight="9315" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25740" windowHeight="9315"/>
   </bookViews>
   <sheets>
-    <sheet name="tagged_result_df" sheetId="1" r:id="rId1"/>
+    <sheet name="tagged_result_df-0.79" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -400,14 +400,14 @@
     <t>VlcCreateTwoPlaylists</t>
   </si>
   <si>
-    <t xml:space="preserve">Average </t>
+    <t>Average</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1352,18 +1352,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A89" workbookViewId="0">
-      <selection activeCell="E120" sqref="E120"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="18.25" customWidth="1"/>
-    <col min="2" max="6" width="9" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -1399,10 +1395,10 @@
         <v>1</v>
       </c>
       <c r="D2">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E2">
-        <v>200.2</v>
+        <v>298.89999999999998</v>
       </c>
       <c r="F2">
         <v>0</v>
@@ -1425,7 +1421,7 @@
         <v>9</v>
       </c>
       <c r="E3">
-        <v>321.3</v>
+        <v>335.4</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -1448,7 +1444,7 @@
         <v>20</v>
       </c>
       <c r="E4">
-        <v>839.9</v>
+        <v>1033.4000000000001</v>
       </c>
       <c r="F4">
         <v>0</v>
@@ -1468,10 +1464,10 @@
         <v>1</v>
       </c>
       <c r="D5">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="E5">
-        <v>608.1</v>
+        <v>1238.5999999999999</v>
       </c>
       <c r="F5">
         <v>0</v>
@@ -1491,10 +1487,10 @@
         <v>0</v>
       </c>
       <c r="D6">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="E6">
-        <v>563.20000000000005</v>
+        <v>1186.3</v>
       </c>
       <c r="F6">
         <v>0</v>
@@ -1514,10 +1510,10 @@
         <v>1</v>
       </c>
       <c r="D7">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E7">
-        <v>59</v>
+        <v>134.30000000000001</v>
       </c>
       <c r="F7">
         <v>0</v>
@@ -1540,7 +1536,7 @@
         <v>6</v>
       </c>
       <c r="E8">
-        <v>129.6</v>
+        <v>185.2</v>
       </c>
       <c r="F8">
         <v>0</v>
@@ -1560,10 +1556,10 @@
         <v>1</v>
       </c>
       <c r="D9">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E9">
-        <v>120.8</v>
+        <v>81.099999999999994</v>
       </c>
       <c r="F9">
         <v>0</v>
@@ -1586,7 +1582,7 @@
         <v>4</v>
       </c>
       <c r="E10">
-        <v>80.599999999999994</v>
+        <v>99.4</v>
       </c>
       <c r="F10">
         <v>0</v>
@@ -1609,7 +1605,7 @@
         <v>9</v>
       </c>
       <c r="E11">
-        <v>217.9</v>
+        <v>646.70000000000005</v>
       </c>
       <c r="F11">
         <v>0</v>
@@ -1629,10 +1625,10 @@
         <v>1</v>
       </c>
       <c r="D12">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E12">
-        <v>223.5</v>
+        <v>314.89999999999998</v>
       </c>
       <c r="F12">
         <v>0</v>
@@ -1652,10 +1648,10 @@
         <v>1</v>
       </c>
       <c r="D13">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E13">
-        <v>308.10000000000002</v>
+        <v>342.6</v>
       </c>
       <c r="F13">
         <v>0</v>
@@ -1675,10 +1671,10 @@
         <v>1</v>
       </c>
       <c r="D14">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="E14">
-        <v>1070.5</v>
+        <v>1549.3</v>
       </c>
       <c r="F14">
         <v>0</v>
@@ -1695,13 +1691,13 @@
         <v>1</v>
       </c>
       <c r="C15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D15">
         <v>31</v>
       </c>
       <c r="E15">
-        <v>869.6</v>
+        <v>1831.8</v>
       </c>
       <c r="F15">
         <v>0</v>
@@ -1721,10 +1717,10 @@
         <v>0</v>
       </c>
       <c r="D16">
-        <v>13</v>
+        <v>60</v>
       </c>
       <c r="E16">
-        <v>347.6</v>
+        <v>2002.4</v>
       </c>
       <c r="F16">
         <v>0</v>
@@ -1744,10 +1740,10 @@
         <v>1</v>
       </c>
       <c r="D17">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E17">
-        <v>290.60000000000002</v>
+        <v>303.60000000000002</v>
       </c>
       <c r="F17">
         <v>0</v>
@@ -1767,10 +1763,10 @@
         <v>1</v>
       </c>
       <c r="D18">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E18">
-        <v>192.2</v>
+        <v>216.1</v>
       </c>
       <c r="F18">
         <v>0</v>
@@ -1787,13 +1783,13 @@
         <v>1</v>
       </c>
       <c r="C19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D19">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="E19">
-        <v>424.3</v>
+        <v>617.20000000000005</v>
       </c>
       <c r="F19">
         <v>0</v>
@@ -1816,7 +1812,7 @@
         <v>11</v>
       </c>
       <c r="E20">
-        <v>225.3</v>
+        <v>301.5</v>
       </c>
       <c r="F20">
         <v>0</v>
@@ -1833,13 +1829,13 @@
         <v>1</v>
       </c>
       <c r="C21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D21">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E21">
-        <v>333.6</v>
+        <v>609.29999999999995</v>
       </c>
       <c r="F21">
         <v>0</v>
@@ -1862,7 +1858,7 @@
         <v>5</v>
       </c>
       <c r="E22">
-        <v>93.2</v>
+        <v>148.4</v>
       </c>
       <c r="F22">
         <v>0</v>
@@ -1882,10 +1878,10 @@
         <v>1</v>
       </c>
       <c r="D23">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E23">
-        <v>670.8</v>
+        <v>1029.5</v>
       </c>
       <c r="F23">
         <v>0</v>
@@ -1902,13 +1898,13 @@
         <v>1</v>
       </c>
       <c r="C24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D24">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="E24">
-        <v>603.5</v>
+        <v>870.7</v>
       </c>
       <c r="F24">
         <v>0</v>
@@ -1925,13 +1921,13 @@
         <v>1</v>
       </c>
       <c r="C25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D25">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E25">
-        <v>431.9</v>
+        <v>359.6</v>
       </c>
       <c r="F25">
         <v>0</v>
@@ -1954,7 +1950,7 @@
         <v>9</v>
       </c>
       <c r="E26">
-        <v>265.60000000000002</v>
+        <v>224.8</v>
       </c>
       <c r="F26">
         <v>0</v>
@@ -1974,10 +1970,10 @@
         <v>1</v>
       </c>
       <c r="D27">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E27">
-        <v>294.2</v>
+        <v>130</v>
       </c>
       <c r="F27">
         <v>0</v>
@@ -2000,7 +1996,7 @@
         <v>10</v>
       </c>
       <c r="E28">
-        <v>244.8</v>
+        <v>712.7</v>
       </c>
       <c r="F28">
         <v>0</v>
@@ -2020,10 +2016,10 @@
         <v>1</v>
       </c>
       <c r="D29">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E29">
-        <v>508.7</v>
+        <v>909.1</v>
       </c>
       <c r="F29">
         <v>0</v>
@@ -2043,10 +2039,10 @@
         <v>1</v>
       </c>
       <c r="D30">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E30">
-        <v>216.1</v>
+        <v>228.8</v>
       </c>
       <c r="F30">
         <v>0</v>
@@ -2066,10 +2062,10 @@
         <v>1</v>
       </c>
       <c r="D31">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E31">
-        <v>143.1</v>
+        <v>592.5</v>
       </c>
       <c r="F31">
         <v>0</v>
@@ -2092,7 +2088,7 @@
         <v>5</v>
       </c>
       <c r="E32">
-        <v>174.2</v>
+        <v>112.2</v>
       </c>
       <c r="F32">
         <v>0</v>
@@ -2115,7 +2111,7 @@
         <v>5</v>
       </c>
       <c r="E33">
-        <v>99.6</v>
+        <v>111.1</v>
       </c>
       <c r="F33">
         <v>0</v>
@@ -2138,7 +2134,7 @@
         <v>7</v>
       </c>
       <c r="E34">
-        <v>158.19999999999999</v>
+        <v>221.6</v>
       </c>
       <c r="F34">
         <v>0</v>
@@ -2158,10 +2154,10 @@
         <v>0</v>
       </c>
       <c r="D35">
-        <v>54</v>
+        <v>29</v>
       </c>
       <c r="E35">
-        <v>1571.9</v>
+        <v>783</v>
       </c>
       <c r="F35">
         <v>0</v>
@@ -2184,7 +2180,7 @@
         <v>10</v>
       </c>
       <c r="E36">
-        <v>262.8</v>
+        <v>604.6</v>
       </c>
       <c r="F36">
         <v>0</v>
@@ -2201,13 +2197,13 @@
         <v>1</v>
       </c>
       <c r="C37">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D37">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="E37">
-        <v>401.1</v>
+        <v>342.8</v>
       </c>
       <c r="F37">
         <v>0</v>
@@ -2230,7 +2226,7 @@
         <v>20</v>
       </c>
       <c r="E38">
-        <v>506.2</v>
+        <v>534.5</v>
       </c>
       <c r="F38">
         <v>0</v>
@@ -2253,7 +2249,7 @@
         <v>5</v>
       </c>
       <c r="E39">
-        <v>94.2</v>
+        <v>115.6</v>
       </c>
       <c r="F39">
         <v>0</v>
@@ -2276,7 +2272,7 @@
         <v>6</v>
       </c>
       <c r="E40">
-        <v>117.8</v>
+        <v>257.2</v>
       </c>
       <c r="F40">
         <v>0</v>
@@ -2296,10 +2292,10 @@
         <v>1</v>
       </c>
       <c r="D41">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E41">
-        <v>119.9</v>
+        <v>212.6</v>
       </c>
       <c r="F41">
         <v>0</v>
@@ -2322,7 +2318,7 @@
         <v>5</v>
       </c>
       <c r="E42">
-        <v>113.3</v>
+        <v>129.6</v>
       </c>
       <c r="F42">
         <v>0</v>
@@ -2345,7 +2341,7 @@
         <v>2</v>
       </c>
       <c r="E43">
-        <v>57</v>
+        <v>42.9</v>
       </c>
       <c r="F43">
         <v>0</v>
@@ -2368,7 +2364,7 @@
         <v>10</v>
       </c>
       <c r="E44">
-        <v>238</v>
+        <v>237.4</v>
       </c>
       <c r="F44">
         <v>0</v>
@@ -2391,7 +2387,7 @@
         <v>6</v>
       </c>
       <c r="E45">
-        <v>120.7</v>
+        <v>140.5</v>
       </c>
       <c r="F45">
         <v>0</v>
@@ -2411,10 +2407,10 @@
         <v>0</v>
       </c>
       <c r="D46">
-        <v>120</v>
+        <v>20</v>
       </c>
       <c r="E46">
-        <v>3411.7</v>
+        <v>456.1</v>
       </c>
       <c r="F46">
         <v>0</v>
@@ -2437,7 +2433,7 @@
         <v>60</v>
       </c>
       <c r="E47">
-        <v>1676.5</v>
+        <v>3535.3</v>
       </c>
       <c r="F47">
         <v>0</v>
@@ -2457,10 +2453,10 @@
         <v>0</v>
       </c>
       <c r="D48">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="E48">
-        <v>1488.9</v>
+        <v>4220.8</v>
       </c>
       <c r="F48">
         <v>0</v>
@@ -2477,13 +2473,13 @@
         <v>1</v>
       </c>
       <c r="C49">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D49">
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="E49">
-        <v>1361</v>
+        <v>3397</v>
       </c>
       <c r="F49">
         <v>0</v>
@@ -2503,10 +2499,10 @@
         <v>0</v>
       </c>
       <c r="D50">
-        <v>60</v>
+        <v>32</v>
       </c>
       <c r="E50">
-        <v>3687.2</v>
+        <v>746.3</v>
       </c>
       <c r="F50">
         <v>0</v>
@@ -2526,10 +2522,10 @@
         <v>1</v>
       </c>
       <c r="D51">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E51">
-        <v>419.7</v>
+        <v>1137.5999999999999</v>
       </c>
       <c r="F51">
         <v>0</v>
@@ -2546,13 +2542,13 @@
         <v>1</v>
       </c>
       <c r="C52">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D52">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E52">
-        <v>148.9</v>
+        <v>477.2</v>
       </c>
       <c r="F52">
         <v>0</v>
@@ -2575,7 +2571,7 @@
         <v>24</v>
       </c>
       <c r="E53">
-        <v>634.29999999999995</v>
+        <v>601.1</v>
       </c>
       <c r="F53">
         <v>0</v>
@@ -2598,7 +2594,7 @@
         <v>34</v>
       </c>
       <c r="E54">
-        <v>868.4</v>
+        <v>764.4</v>
       </c>
       <c r="F54">
         <v>0</v>
@@ -2621,7 +2617,7 @@
         <v>14</v>
       </c>
       <c r="E55">
-        <v>333.2</v>
+        <v>301.8</v>
       </c>
       <c r="F55">
         <v>0</v>
@@ -2641,10 +2637,10 @@
         <v>1</v>
       </c>
       <c r="D56">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E56">
-        <v>85.8</v>
+        <v>105.9</v>
       </c>
       <c r="F56">
         <v>0</v>
@@ -2664,10 +2660,10 @@
         <v>1</v>
       </c>
       <c r="D57">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="E57">
-        <v>423.1</v>
+        <v>940.6</v>
       </c>
       <c r="F57">
         <v>0</v>
@@ -2690,7 +2686,7 @@
         <v>6</v>
       </c>
       <c r="E58">
-        <v>122</v>
+        <v>123.3</v>
       </c>
       <c r="F58">
         <v>0</v>
@@ -2710,10 +2706,10 @@
         <v>1</v>
       </c>
       <c r="D59">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E59">
-        <v>180.3</v>
+        <v>152.80000000000001</v>
       </c>
       <c r="F59">
         <v>0</v>
@@ -2733,10 +2729,10 @@
         <v>1</v>
       </c>
       <c r="D60">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E60">
-        <v>467.2</v>
+        <v>475.6</v>
       </c>
       <c r="F60">
         <v>0</v>
@@ -2756,10 +2752,10 @@
         <v>1</v>
       </c>
       <c r="D61">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E61">
-        <v>649.20000000000005</v>
+        <v>931.6</v>
       </c>
       <c r="F61">
         <v>0</v>
@@ -2782,7 +2778,7 @@
         <v>30</v>
       </c>
       <c r="E62">
-        <v>787.6</v>
+        <v>756.5</v>
       </c>
       <c r="F62">
         <v>0</v>
@@ -2802,10 +2798,10 @@
         <v>1</v>
       </c>
       <c r="D63">
-        <v>39</v>
+        <v>24</v>
       </c>
       <c r="E63">
-        <v>999.6</v>
+        <v>562.9</v>
       </c>
       <c r="F63">
         <v>0</v>
@@ -2822,13 +2818,13 @@
         <v>1</v>
       </c>
       <c r="C64">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D64">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="E64">
-        <v>403</v>
+        <v>159</v>
       </c>
       <c r="F64">
         <v>0</v>
@@ -2851,7 +2847,7 @@
         <v>15</v>
       </c>
       <c r="E65">
-        <v>391.8</v>
+        <v>409</v>
       </c>
       <c r="F65">
         <v>0</v>
@@ -2871,10 +2867,10 @@
         <v>1</v>
       </c>
       <c r="D66">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E66">
-        <v>507</v>
+        <v>537.5</v>
       </c>
       <c r="F66">
         <v>0</v>
@@ -2897,7 +2893,7 @@
         <v>18</v>
       </c>
       <c r="E67">
-        <v>464.5</v>
+        <v>464.9</v>
       </c>
       <c r="F67">
         <v>0</v>
@@ -2917,10 +2913,10 @@
         <v>1</v>
       </c>
       <c r="D68">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E68">
-        <v>515.79999999999995</v>
+        <v>397</v>
       </c>
       <c r="F68">
         <v>0</v>
@@ -2937,13 +2933,13 @@
         <v>1</v>
       </c>
       <c r="C69">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D69">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E69">
-        <v>578.79999999999995</v>
+        <v>427.7</v>
       </c>
       <c r="F69">
         <v>0</v>
@@ -2963,10 +2959,10 @@
         <v>1</v>
       </c>
       <c r="D70">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="E70">
-        <v>253.7</v>
+        <v>94.4</v>
       </c>
       <c r="F70">
         <v>0</v>
@@ -2989,7 +2985,7 @@
         <v>12</v>
       </c>
       <c r="E71">
-        <v>334.1</v>
+        <v>321.2</v>
       </c>
       <c r="F71">
         <v>0</v>
@@ -3012,7 +3008,7 @@
         <v>9</v>
       </c>
       <c r="E72">
-        <v>237.8</v>
+        <v>218.1</v>
       </c>
       <c r="F72">
         <v>0</v>
@@ -3035,7 +3031,7 @@
         <v>6</v>
       </c>
       <c r="E73">
-        <v>184.6</v>
+        <v>141</v>
       </c>
       <c r="F73">
         <v>0</v>
@@ -3058,7 +3054,7 @@
         <v>4</v>
       </c>
       <c r="E74">
-        <v>114.3</v>
+        <v>95</v>
       </c>
       <c r="F74">
         <v>0</v>
@@ -3075,13 +3071,13 @@
         <v>1</v>
       </c>
       <c r="C75">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D75">
         <v>10</v>
       </c>
       <c r="E75">
-        <v>433.9</v>
+        <v>267.5</v>
       </c>
       <c r="F75">
         <v>0</v>
@@ -3098,13 +3094,13 @@
         <v>1</v>
       </c>
       <c r="C76">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D76">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="E76">
-        <v>291.8</v>
+        <v>101.2</v>
       </c>
       <c r="F76">
         <v>0</v>
@@ -3127,7 +3123,7 @@
         <v>4</v>
       </c>
       <c r="E77">
-        <v>99.1</v>
+        <v>87.8</v>
       </c>
       <c r="F77">
         <v>0</v>
@@ -3147,10 +3143,10 @@
         <v>1</v>
       </c>
       <c r="D78">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E78">
-        <v>99.8</v>
+        <v>159</v>
       </c>
       <c r="F78">
         <v>0</v>
@@ -3170,10 +3166,10 @@
         <v>1</v>
       </c>
       <c r="D79">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E79">
-        <v>217</v>
+        <v>120.2</v>
       </c>
       <c r="F79">
         <v>0</v>
@@ -3190,13 +3186,13 @@
         <v>1</v>
       </c>
       <c r="C80">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D80">
         <v>4</v>
       </c>
       <c r="E80">
-        <v>98.1</v>
+        <v>102.2</v>
       </c>
       <c r="F80">
         <v>0</v>
@@ -3216,10 +3212,10 @@
         <v>1</v>
       </c>
       <c r="D81">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E81">
-        <v>325.2</v>
+        <v>126.8</v>
       </c>
       <c r="F81">
         <v>0</v>
@@ -3239,10 +3235,10 @@
         <v>1</v>
       </c>
       <c r="D82">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E82">
-        <v>294.89999999999998</v>
+        <v>603.70000000000005</v>
       </c>
       <c r="F82">
         <v>0</v>
@@ -3265,7 +3261,7 @@
         <v>6</v>
       </c>
       <c r="E83">
-        <v>204.3</v>
+        <v>149.30000000000001</v>
       </c>
       <c r="F83">
         <v>0</v>
@@ -3288,7 +3284,7 @@
         <v>6</v>
       </c>
       <c r="E84">
-        <v>166.1</v>
+        <v>158.19999999999999</v>
       </c>
       <c r="F84">
         <v>0</v>
@@ -3311,7 +3307,7 @@
         <v>6</v>
       </c>
       <c r="E85">
-        <v>193.3</v>
+        <v>145.5</v>
       </c>
       <c r="F85">
         <v>0</v>
@@ -3334,7 +3330,7 @@
         <v>9</v>
       </c>
       <c r="E86">
-        <v>389.8</v>
+        <v>187</v>
       </c>
       <c r="F86">
         <v>0</v>
@@ -3354,10 +3350,10 @@
         <v>1</v>
       </c>
       <c r="D87">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E87">
-        <v>267</v>
+        <v>224.2</v>
       </c>
       <c r="F87">
         <v>0</v>
@@ -3377,10 +3373,10 @@
         <v>1</v>
       </c>
       <c r="D88">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E88">
-        <v>430.4</v>
+        <v>306.2</v>
       </c>
       <c r="F88">
         <v>0</v>
@@ -3400,10 +3396,10 @@
         <v>1</v>
       </c>
       <c r="D89">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E89">
-        <v>78.599999999999994</v>
+        <v>112.4</v>
       </c>
       <c r="F89">
         <v>0</v>
@@ -3426,7 +3422,7 @@
         <v>4</v>
       </c>
       <c r="E90">
-        <v>102.4</v>
+        <v>98.1</v>
       </c>
       <c r="F90">
         <v>0</v>
@@ -3443,13 +3439,13 @@
         <v>1</v>
       </c>
       <c r="C91">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D91">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="E91">
-        <v>77.2</v>
+        <v>348.7</v>
       </c>
       <c r="F91">
         <v>0</v>
@@ -3466,13 +3462,13 @@
         <v>1</v>
       </c>
       <c r="C92">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D92">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E92">
-        <v>81.7</v>
+        <v>112.6</v>
       </c>
       <c r="F92">
         <v>0</v>
@@ -3489,13 +3485,13 @@
         <v>1</v>
       </c>
       <c r="C93">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D93">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="E93">
-        <v>399.2</v>
+        <v>121.3</v>
       </c>
       <c r="F93">
         <v>0</v>
@@ -3512,13 +3508,13 @@
         <v>1</v>
       </c>
       <c r="C94">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D94">
         <v>3</v>
       </c>
       <c r="E94">
-        <v>87.2</v>
+        <v>283.7</v>
       </c>
       <c r="F94">
         <v>0</v>
@@ -3541,7 +3537,7 @@
         <v>5</v>
       </c>
       <c r="E95">
-        <v>105.2</v>
+        <v>192.2</v>
       </c>
       <c r="F95">
         <v>0</v>
@@ -3564,7 +3560,7 @@
         <v>5</v>
       </c>
       <c r="E96">
-        <v>108.8</v>
+        <v>88.2</v>
       </c>
       <c r="F96">
         <v>0</v>
@@ -3587,7 +3583,7 @@
         <v>6</v>
       </c>
       <c r="E97">
-        <v>123.9</v>
+        <v>119.4</v>
       </c>
       <c r="F97">
         <v>0</v>
@@ -3610,7 +3606,7 @@
         <v>6</v>
       </c>
       <c r="E98">
-        <v>130.69999999999999</v>
+        <v>109.4</v>
       </c>
       <c r="F98">
         <v>0</v>
@@ -3630,10 +3626,10 @@
         <v>1</v>
       </c>
       <c r="D99">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E99">
-        <v>154.80000000000001</v>
+        <v>123</v>
       </c>
       <c r="F99">
         <v>0</v>
@@ -3656,7 +3652,7 @@
         <v>4</v>
       </c>
       <c r="E100">
-        <v>82.5</v>
+        <v>79.599999999999994</v>
       </c>
       <c r="F100">
         <v>0</v>
@@ -3679,7 +3675,7 @@
         <v>6</v>
       </c>
       <c r="E101">
-        <v>184.8</v>
+        <v>121.2</v>
       </c>
       <c r="F101">
         <v>0</v>
@@ -3699,10 +3695,10 @@
         <v>1</v>
       </c>
       <c r="D102">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E102">
-        <v>142.5</v>
+        <v>76.3</v>
       </c>
       <c r="F102">
         <v>0</v>
@@ -3725,7 +3721,7 @@
         <v>6</v>
       </c>
       <c r="E103">
-        <v>176.6</v>
+        <v>147.80000000000001</v>
       </c>
       <c r="F103">
         <v>0</v>
@@ -3748,7 +3744,7 @@
         <v>5</v>
       </c>
       <c r="E104">
-        <v>106.2</v>
+        <v>117.3</v>
       </c>
       <c r="F104">
         <v>0</v>
@@ -3771,7 +3767,7 @@
         <v>4</v>
       </c>
       <c r="E105">
-        <v>88.4</v>
+        <v>79.900000000000006</v>
       </c>
       <c r="F105">
         <v>0</v>
@@ -3794,7 +3790,7 @@
         <v>5</v>
       </c>
       <c r="E106">
-        <v>126.9</v>
+        <v>99.3</v>
       </c>
       <c r="F106">
         <v>0</v>
@@ -3817,7 +3813,7 @@
         <v>4</v>
       </c>
       <c r="E107">
-        <v>79.7</v>
+        <v>86</v>
       </c>
       <c r="F107">
         <v>0</v>
@@ -3840,7 +3836,7 @@
         <v>4</v>
       </c>
       <c r="E108">
-        <v>129.5</v>
+        <v>90.5</v>
       </c>
       <c r="F108">
         <v>0</v>
@@ -3860,10 +3856,10 @@
         <v>0</v>
       </c>
       <c r="D109">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="E109">
-        <v>54.1</v>
+        <v>281.10000000000002</v>
       </c>
       <c r="F109">
         <v>0</v>
@@ -3883,10 +3879,10 @@
         <v>1</v>
       </c>
       <c r="D110">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E110">
-        <v>114.2</v>
+        <v>80.5</v>
       </c>
       <c r="F110">
         <v>0</v>
@@ -3909,7 +3905,7 @@
         <v>3</v>
       </c>
       <c r="E111">
-        <v>96.2</v>
+        <v>68</v>
       </c>
       <c r="F111">
         <v>0</v>
@@ -3932,7 +3928,7 @@
         <v>3</v>
       </c>
       <c r="E112">
-        <v>70</v>
+        <v>60.5</v>
       </c>
       <c r="F112">
         <v>0</v>
@@ -3955,7 +3951,7 @@
         <v>3</v>
       </c>
       <c r="E113">
-        <v>77</v>
+        <v>65.5</v>
       </c>
       <c r="F113">
         <v>0</v>
@@ -3978,7 +3974,7 @@
         <v>11</v>
       </c>
       <c r="E114">
-        <v>268.8</v>
+        <v>207.2</v>
       </c>
       <c r="F114">
         <v>0</v>
@@ -3998,10 +3994,10 @@
         <v>1</v>
       </c>
       <c r="D115">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E115">
-        <v>175</v>
+        <v>100.9</v>
       </c>
       <c r="F115">
         <v>0</v>
@@ -4021,10 +4017,10 @@
         <v>0</v>
       </c>
       <c r="D116">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="E116">
-        <v>702.7</v>
+        <v>280.10000000000002</v>
       </c>
       <c r="F116">
         <v>0</v>
@@ -4047,7 +4043,7 @@
         <v>48</v>
       </c>
       <c r="E117">
-        <v>514.6</v>
+        <v>1317.5</v>
       </c>
       <c r="F117">
         <v>0</v>
@@ -4061,19 +4057,24 @@
         <v>126</v>
       </c>
       <c r="B118">
+        <f t="shared" ref="B118:F118" si="0">AVERAGE(B2:B117)</f>
         <v>1</v>
       </c>
       <c r="C118">
-        <f>AVERAGE(C2:C117)</f>
-        <v>0.75</v>
+        <f t="shared" si="0"/>
+        <v>0.7931034482758621</v>
       </c>
       <c r="D118">
-        <f>AVERAGE(D2:D117)</f>
-        <v>13.646551724137931</v>
+        <f t="shared" si="0"/>
+        <v>12.258620689655173</v>
       </c>
       <c r="E118">
-        <f>AVERAGE(E2:E117)</f>
-        <v>386.31724137931036</v>
+        <f t="shared" si="0"/>
+        <v>458.0887931034481</v>
+      </c>
+      <c r="F118">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>